<commit_message>
fix: Add purpose in Readme
</commit_message>
<xml_diff>
--- a/task1/Result/res_f1/table_of_all_results.xlsx
+++ b/task1/Result/res_f1/table_of_all_results.xlsx
@@ -4,7 +4,7 @@
   <x:fileVersion appName="HCell" lastEdited="9.6" lowestEdited="9.6" rupBuild="1.8005"/>
   <x:workbookPr date1904="0" showBorderUnselectedTables="1" filterPrivacy="0" promptedSolutions="0" showInkAnnotation="1" backupFile="0" saveExternalLinkValues="1" codeName="ЭтаКнига" hidePivotFieldList="0" allowRefreshQuery="0" publishItems="0" checkCompatibility="0" autoCompressPictures="1" refreshAllConnections="0"/>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="16860" windowHeight="5820"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="16860" windowHeight="5928"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Лист1" sheetId="1" r:id="rId4"/>
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="15">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="17">
   <x:si>
     <x:t>N</x:t>
+  </x:si>
+  <x:si>
+    <x:t>S</x:t>
   </x:si>
   <x:si>
     <x:t>Time (sec)</x:t>
@@ -28,37 +31,40 @@
     <x:t>Среднее значение</x:t>
   </x:si>
   <x:si>
+    <x:t>Ускорение</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Экс 6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Thread</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Экс 9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Экс 8</x:t>
+  </x:si>
+  <x:si>
     <x:t>Экс 10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Экс 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Экс 1</x:t>
   </x:si>
   <x:si>
     <x:t>Экс 4</x:t>
   </x:si>
   <x:si>
-    <x:t>Экс 3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Экс 8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Экс 9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Экс 2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Экс 1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Thread</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Экс 6</x:t>
+    <x:t>Экс 5</x:t>
   </x:si>
   <x:si>
     <x:t>Экс 7</x:t>
   </x:si>
   <x:si>
-    <x:t>Экс 5</x:t>
+    <x:t>Экс 2</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -110,7 +116,7 @@
       <x:patternFill patternType="gray125"/>
     </x:fill>
   </x:fills>
-  <x:borders count="17">
+  <x:borders count="25">
     <x:border>
       <x:left>
         <x:color indexed="64"/>
@@ -349,6 +355,118 @@
         <x:color rgb="ffff0303"/>
       </x:bottom>
     </x:border>
+    <x:border>
+      <x:left style="medium">
+        <x:color rgb="ff000000"/>
+      </x:left>
+      <x:right>
+        <x:color rgb="ff000000"/>
+      </x:right>
+      <x:top style="medium">
+        <x:color rgb="ff000000"/>
+      </x:top>
+      <x:bottom>
+        <x:color rgb="ff000000"/>
+      </x:bottom>
+    </x:border>
+    <x:border>
+      <x:left>
+        <x:color rgb="ff000000"/>
+      </x:left>
+      <x:right>
+        <x:color rgb="ff000000"/>
+      </x:right>
+      <x:top style="medium">
+        <x:color rgb="ff000000"/>
+      </x:top>
+      <x:bottom>
+        <x:color rgb="ff000000"/>
+      </x:bottom>
+    </x:border>
+    <x:border>
+      <x:left>
+        <x:color rgb="ff000000"/>
+      </x:left>
+      <x:right style="medium">
+        <x:color rgb="ff000000"/>
+      </x:right>
+      <x:top style="medium">
+        <x:color rgb="ff000000"/>
+      </x:top>
+      <x:bottom>
+        <x:color rgb="ff000000"/>
+      </x:bottom>
+    </x:border>
+    <x:border>
+      <x:left style="medium">
+        <x:color rgb="ff000000"/>
+      </x:left>
+      <x:right>
+        <x:color rgb="ff000000"/>
+      </x:right>
+      <x:top>
+        <x:color rgb="ff000000"/>
+      </x:top>
+      <x:bottom>
+        <x:color rgb="ff000000"/>
+      </x:bottom>
+    </x:border>
+    <x:border>
+      <x:left>
+        <x:color rgb="ff000000"/>
+      </x:left>
+      <x:right style="medium">
+        <x:color rgb="ff000000"/>
+      </x:right>
+      <x:top>
+        <x:color rgb="ff000000"/>
+      </x:top>
+      <x:bottom>
+        <x:color rgb="ff000000"/>
+      </x:bottom>
+    </x:border>
+    <x:border>
+      <x:left style="medium">
+        <x:color rgb="ff000000"/>
+      </x:left>
+      <x:right>
+        <x:color rgb="ff000000"/>
+      </x:right>
+      <x:top>
+        <x:color rgb="ff000000"/>
+      </x:top>
+      <x:bottom style="medium">
+        <x:color rgb="ff000000"/>
+      </x:bottom>
+    </x:border>
+    <x:border>
+      <x:left>
+        <x:color rgb="ff000000"/>
+      </x:left>
+      <x:right>
+        <x:color rgb="ff000000"/>
+      </x:right>
+      <x:top>
+        <x:color rgb="ff000000"/>
+      </x:top>
+      <x:bottom style="medium">
+        <x:color rgb="ff000000"/>
+      </x:bottom>
+    </x:border>
+    <x:border>
+      <x:left>
+        <x:color rgb="ff000000"/>
+      </x:left>
+      <x:right style="medium">
+        <x:color rgb="ff000000"/>
+      </x:right>
+      <x:top>
+        <x:color rgb="ff000000"/>
+      </x:top>
+      <x:bottom style="medium">
+        <x:color rgb="ff000000"/>
+      </x:bottom>
+    </x:border>
   </x:borders>
   <x:cellStyleXfs count="20">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -412,7 +530,7 @@
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="21">
+  <x:cellXfs count="29">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <x:alignment horizontal="general" vertical="bottom"/>
     </x:xf>
@@ -474,6 +592,30 @@
       <x:alignment horizontal="left" vertical="bottom"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="left" vertical="bottom"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1">
+      <x:alignment horizontal="general" vertical="bottom"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
+      <x:alignment horizontal="general" vertical="bottom"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1">
+      <x:alignment horizontal="general" vertical="bottom"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1">
+      <x:alignment horizontal="general" vertical="bottom"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="left" vertical="bottom"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1">
+      <x:alignment horizontal="general" vertical="bottom"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="left" vertical="bottom"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <x:alignment horizontal="left" vertical="bottom"/>
     </x:xf>
   </x:cellXfs>
@@ -1186,7 +1328,7 @@
   <x:dimension ref="B2:L121"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="A1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="L20" activeCellId="0" sqref="L20:L20"/>
+      <x:selection activeCell="K16" activeCellId="0" sqref="K16:K16"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.199999999999999"/>
@@ -1202,14 +1344,14 @@
   <x:sheetData>
     <x:row r="2" spans="2:12" ht="14.550000000000001">
       <x:c r="B2" s="12" t="s">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="C2" s="13"/>
       <x:c r="D2" s="13"/>
       <x:c r="E2" s="13"/>
       <x:c r="F2" s="14"/>
       <x:c r="H2" s="1" t="s">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="I2" s="2"/>
       <x:c r="J2" s="2"/>
@@ -1222,26 +1364,26 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D3" s="5" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="E3" s="5" t="s">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="F3" s="16" t="s">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="H3" s="4"/>
       <x:c r="I3" s="5" t="s">
         <x:v>0</x:v>
       </x:c>
       <x:c r="J3" s="5" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="K3" s="5" t="s">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="L3" s="6" t="s">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="2:12">
@@ -1536,7 +1678,7 @@
     </x:row>
     <x:row r="14" spans="2:6">
       <x:c r="B14" s="15" t="s">
-        <x:v>9</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C14" s="11"/>
       <x:c r="D14" s="11"/>
@@ -1549,17 +1691,19 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D15" s="5" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="E15" s="5" t="s">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="F15" s="16" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="H15" s="11"/>
-      <x:c r="I15" s="11"/>
-      <x:c r="J15" s="11"/>
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="H15" s="21" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="I15" s="22"/>
+      <x:c r="J15" s="23"/>
     </x:row>
     <x:row r="16" spans="2:10">
       <x:c r="B16" s="15"/>
@@ -1575,9 +1719,13 @@
       <x:c r="F16" s="16">
         <x:v>1658</x:v>
       </x:c>
-      <x:c r="H16" s="11"/>
-      <x:c r="I16" s="5"/>
-      <x:c r="J16" s="5"/>
+      <x:c r="H16" s="24"/>
+      <x:c r="I16" s="5" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="J16" s="25" t="s">
+        <x:v>1</x:v>
+      </x:c>
     </x:row>
     <x:row r="17" spans="2:10">
       <x:c r="B17" s="15"/>
@@ -1593,9 +1741,14 @@
       <x:c r="F17" s="16">
         <x:v>2636</x:v>
       </x:c>
-      <x:c r="H17" s="11"/>
-      <x:c r="I17" s="5"/>
-      <x:c r="J17" s="5"/>
+      <x:c r="H17" s="24"/>
+      <x:c r="I17" s="5">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="J17" s="25">
+        <x:f>K4/K9</x:f>
+        <x:v>1.0207371797939175</x:v>
+      </x:c>
     </x:row>
     <x:row r="18" spans="2:10">
       <x:c r="B18" s="15"/>
@@ -1611,9 +1764,14 @@
       <x:c r="F18" s="16">
         <x:v>3122</x:v>
       </x:c>
-      <x:c r="H18" s="11"/>
-      <x:c r="I18" s="5"/>
-      <x:c r="J18" s="5"/>
+      <x:c r="H18" s="24"/>
+      <x:c r="I18" s="5">
+        <x:v>300</x:v>
+      </x:c>
+      <x:c r="J18" s="25">
+        <x:f>K5/K10</x:f>
+        <x:v>1.6372834141484742</x:v>
+      </x:c>
     </x:row>
     <x:row r="19" spans="2:10">
       <x:c r="B19" s="15"/>
@@ -1629,9 +1787,14 @@
       <x:c r="F19" s="16">
         <x:v>3673</x:v>
       </x:c>
-      <x:c r="H19" s="11"/>
-      <x:c r="I19" s="5"/>
-      <x:c r="J19" s="5"/>
+      <x:c r="H19" s="24"/>
+      <x:c r="I19" s="5">
+        <x:v>500</x:v>
+      </x:c>
+      <x:c r="J19" s="25">
+        <x:f>K6/K11</x:f>
+        <x:v>1.5229614646458021</x:v>
+      </x:c>
     </x:row>
     <x:row r="20" spans="2:10">
       <x:c r="B20" s="15"/>
@@ -1647,9 +1810,14 @@
       <x:c r="F20" s="16">
         <x:v>4183</x:v>
       </x:c>
-      <x:c r="H20" s="11"/>
-      <x:c r="I20" s="5"/>
-      <x:c r="J20" s="5"/>
+      <x:c r="H20" s="24"/>
+      <x:c r="I20" s="5">
+        <x:v>1000</x:v>
+      </x:c>
+      <x:c r="J20" s="25">
+        <x:f>K7/K12</x:f>
+        <x:v>2.0105758450477884</x:v>
+      </x:c>
     </x:row>
     <x:row r="21" spans="2:10" ht="14.550000000000001">
       <x:c r="B21" s="15"/>
@@ -1665,9 +1833,14 @@
       <x:c r="F21" s="16">
         <x:v>1658</x:v>
       </x:c>
-      <x:c r="H21" s="11"/>
-      <x:c r="I21" s="5"/>
-      <x:c r="J21" s="5"/>
+      <x:c r="H21" s="26"/>
+      <x:c r="I21" s="27">
+        <x:v>3000</x:v>
+      </x:c>
+      <x:c r="J21" s="28">
+        <x:f>K8/K13</x:f>
+        <x:v>2.1578092648387899</x:v>
+      </x:c>
     </x:row>
     <x:row r="22" spans="2:6">
       <x:c r="B22" s="15"/>
@@ -1731,7 +1904,7 @@
     </x:row>
     <x:row r="26" spans="2:6">
       <x:c r="B26" s="15" t="s">
-        <x:v>6</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="C26" s="11"/>
       <x:c r="D26" s="11"/>
@@ -1744,13 +1917,13 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D27" s="5" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="E27" s="5" t="s">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="F27" s="16" t="s">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="2:6">
@@ -1905,7 +2078,7 @@
     </x:row>
     <x:row r="38" spans="2:6">
       <x:c r="B38" s="15" t="s">
-        <x:v>5</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C38" s="11"/>
       <x:c r="D38" s="11"/>
@@ -1918,13 +2091,13 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D39" s="5" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="E39" s="5" t="s">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="F39" s="16" t="s">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="2:6">
@@ -2092,13 +2265,13 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D51" s="5" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="E51" s="5" t="s">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="F51" s="16" t="s">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="2:6">
@@ -2253,7 +2426,7 @@
     </x:row>
     <x:row r="62" spans="2:6">
       <x:c r="B62" s="15" t="s">
-        <x:v>12</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="C62" s="11"/>
       <x:c r="D62" s="11"/>
@@ -2266,13 +2439,13 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D63" s="5" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="E63" s="5" t="s">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="F63" s="16" t="s">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="64" spans="2:6">
@@ -2427,7 +2600,7 @@
     </x:row>
     <x:row r="74" spans="2:6">
       <x:c r="B74" s="15" t="s">
-        <x:v>13</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C74" s="11"/>
       <x:c r="D74" s="11"/>
@@ -2440,13 +2613,13 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D75" s="5" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="E75" s="5" t="s">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="F75" s="16" t="s">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="76" spans="2:6">
@@ -2601,7 +2774,7 @@
     </x:row>
     <x:row r="86" spans="2:6">
       <x:c r="B86" s="15" t="s">
-        <x:v>7</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C86" s="11"/>
       <x:c r="D86" s="11"/>
@@ -2614,13 +2787,13 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D87" s="5" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="E87" s="5" t="s">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="F87" s="16" t="s">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="88" spans="2:6">
@@ -2788,13 +2961,13 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D99" s="5" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="E99" s="5" t="s">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="F99" s="16" t="s">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="100" spans="2:6">
@@ -2949,7 +3122,7 @@
     </x:row>
     <x:row r="110" spans="2:6">
       <x:c r="B110" s="15" t="s">
-        <x:v>4</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C110" s="11"/>
       <x:c r="D110" s="11"/>
@@ -2962,13 +3135,13 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="D111" s="5" t="s">
-        <x:v>11</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="E111" s="5" t="s">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="F111" s="16" t="s">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="112" spans="2:6">

</xml_diff>

<commit_message>
feat: Add confidence interval
</commit_message>
<xml_diff>
--- a/task1/Result/res_f1/table_of_all_results.xlsx
+++ b/task1/Result/res_f1/table_of_all_results.xlsx
@@ -4,7 +4,7 @@
   <x:fileVersion appName="HCell" lastEdited="9.6" lowestEdited="9.6" rupBuild="1.8005"/>
   <x:workbookPr date1904="0" showBorderUnselectedTables="1" filterPrivacy="0" promptedSolutions="0" showInkAnnotation="1" backupFile="0" saveExternalLinkValues="1" codeName="ЭтаКнига" hidePivotFieldList="0" allowRefreshQuery="0" publishItems="0" checkCompatibility="0" autoCompressPictures="1" refreshAllConnections="0"/>
   <x:bookViews>
-    <x:workbookView xWindow="0" yWindow="0" windowWidth="16860" windowHeight="5928"/>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="22644" windowHeight="8892"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Лист1" sheetId="1" r:id="rId4"/>
@@ -14,12 +14,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="17">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="19">
+  <x:si>
+    <x:t>Среднее значение</x:t>
+  </x:si>
   <x:si>
     <x:t>N</x:t>
   </x:si>
   <x:si>
     <x:t>S</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Дисперсия</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Погрешность</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ускорение</x:t>
   </x:si>
   <x:si>
     <x:t>Time (sec)</x:t>
@@ -28,10 +40,19 @@
     <x:t>Iteration</x:t>
   </x:si>
   <x:si>
-    <x:t>Среднее значение</x:t>
+    <x:t>Экс 2</x:t>
   </x:si>
   <x:si>
-    <x:t>Ускорение</x:t>
+    <x:t>Экс 5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Экс 9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Экс 3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Экс 10</x:t>
   </x:si>
   <x:si>
     <x:t>Экс 6</x:t>
@@ -40,16 +61,7 @@
     <x:t>Thread</x:t>
   </x:si>
   <x:si>
-    <x:t>Экс 9</x:t>
-  </x:si>
-  <x:si>
     <x:t>Экс 8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Экс 10</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Экс 3</x:t>
   </x:si>
   <x:si>
     <x:t>Экс 1</x:t>
@@ -58,13 +70,7 @@
     <x:t>Экс 4</x:t>
   </x:si>
   <x:si>
-    <x:t>Экс 5</x:t>
-  </x:si>
-  <x:si>
     <x:t>Экс 7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Экс 2</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -530,7 +536,7 @@
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="29">
+  <x:cellXfs count="32">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <x:alignment horizontal="general" vertical="bottom"/>
     </x:xf>
@@ -616,6 +622,15 @@
       <x:alignment horizontal="left" vertical="bottom"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="left" vertical="bottom"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="left" vertical="bottom"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <x:alignment horizontal="left" vertical="bottom"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <x:alignment horizontal="left" vertical="bottom"/>
     </x:xf>
   </x:cellXfs>
@@ -1325,10 +1340,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr codeName="Лист1"/>
-  <x:dimension ref="B2:L121"/>
+  <x:dimension ref="B2:Q121"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" topLeftCell="A1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <x:selection activeCell="K16" activeCellId="0" sqref="K16:K16"/>
+      <x:selection activeCell="R16" activeCellId="0" sqref="R16:R16"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.199999999999999"/>
@@ -1340,53 +1355,69 @@
     <x:col min="7" max="7" width="11.22265625" customWidth="1"/>
     <x:col min="8" max="8" width="16.77734375" customWidth="1"/>
     <x:col min="10" max="10" width="13.0859375" bestFit="1" customWidth="1"/>
+    <x:col min="13" max="13" width="6" customWidth="1"/>
+    <x:col min="14" max="14" width="8.33203125" customWidth="1"/>
+    <x:col min="16" max="16" width="15.33203125" customWidth="1"/>
+    <x:col min="17" max="17" width="15.77734375" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="2" spans="2:12" ht="14.550000000000001">
       <x:c r="B2" s="12" t="s">
-        <x:v>12</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C2" s="13"/>
       <x:c r="D2" s="13"/>
       <x:c r="E2" s="13"/>
       <x:c r="F2" s="14"/>
       <x:c r="H2" s="1" t="s">
-        <x:v>4</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="I2" s="2"/>
       <x:c r="J2" s="2"/>
       <x:c r="K2" s="2"/>
       <x:c r="L2" s="3"/>
     </x:row>
-    <x:row r="3" spans="2:12">
+    <x:row r="3" spans="2:17" ht="14.550000000000001">
       <x:c r="B3" s="15"/>
       <x:c r="C3" s="5" t="s">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="D3" s="5" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E3" s="5" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="F3" s="16" t="s">
         <x:v>7</x:v>
-      </x:c>
-      <x:c r="E3" s="5" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="F3" s="16" t="s">
-        <x:v>3</x:v>
       </x:c>
       <x:c r="H3" s="4"/>
       <x:c r="I3" s="5" t="s">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="J3" s="5" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="K3" s="5" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="L3" s="6" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="K3" s="5" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="L3" s="6" t="s">
+      <x:c r="N3" s="29" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="O3" s="30" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="P3" s="1" t="s">
         <x:v>3</x:v>
       </x:c>
-    </x:row>
-    <x:row r="4" spans="2:12">
+      <x:c r="Q3" s="3" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="2:17">
       <x:c r="B4" s="15"/>
       <x:c r="C4" s="5">
         <x:v>100</x:v>
@@ -1414,8 +1445,22 @@
       <x:c r="L4" s="6">
         <x:v>1658</x:v>
       </x:c>
-    </x:row>
-    <x:row r="5" spans="2:12">
+      <x:c r="N4" s="7">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="O4" s="5">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="P4" s="7">
+        <x:f>SQRT(SUMSQ(E4-K4,E16-K4,E28-K4,E40-K4,E52-K4,E64-K4,E76-K4,E88-K4,E100-K4,E112-K4))/10</x:f>
+        <x:v>0.009915893273981926</x:v>
+      </x:c>
+      <x:c r="Q4" s="6">
+        <x:f>1.96*(P4/SQRT(10))</x:f>
+        <x:v>0.0061459343250616786</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="2:17">
       <x:c r="B5" s="15"/>
       <x:c r="C5" s="5">
         <x:v>300</x:v>
@@ -1443,8 +1488,22 @@
       <x:c r="L5" s="6">
         <x:v>2636</x:v>
       </x:c>
-    </x:row>
-    <x:row r="6" spans="2:12">
+      <x:c r="N5" s="7">
+        <x:v>300</x:v>
+      </x:c>
+      <x:c r="O5" s="5">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="P5" s="7">
+        <x:f t="shared" ref="P5:P13" si="1">SQRT(SUMSQ(E5-K5,E17-K5,E29-K5,E41-K5,E53-K5,E65-K5,E77-K5,E89-K5,E101-K5,E113-K5))/10</x:f>
+        <x:v>0.11673344738521174</x:v>
+      </x:c>
+      <x:c r="Q5" s="6">
+        <x:f t="shared" ref="Q5:Q13" si="2">1.96*(P5/SQRT(10))</x:f>
+        <x:v>0.07235214028069642</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="2:17">
       <x:c r="B6" s="15"/>
       <x:c r="C6" s="5">
         <x:v>500</x:v>
@@ -1472,8 +1531,22 @@
       <x:c r="L6" s="6">
         <x:v>3122</x:v>
       </x:c>
-    </x:row>
-    <x:row r="7" spans="2:12">
+      <x:c r="N6" s="7">
+        <x:v>500</x:v>
+      </x:c>
+      <x:c r="O6" s="5">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="P6" s="7">
+        <x:f>SQRT(SUMSQ(E6-K6,E18-K6,E30-K6,E42-K6,E54-K6,E66-K6,E78-K6,E90-K6,E102-K6,E114-K6))/10</x:f>
+        <x:v>0.23676769270410189</x:v>
+      </x:c>
+      <x:c r="Q6" s="6">
+        <x:f t="shared" si="2"/>
+        <x:v>0.14675013631640746</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="2:17">
       <x:c r="B7" s="15"/>
       <x:c r="C7" s="5">
         <x:v>1000</x:v>
@@ -1501,8 +1574,22 @@
       <x:c r="L7" s="6">
         <x:v>3673</x:v>
       </x:c>
-    </x:row>
-    <x:row r="8" spans="2:12">
+      <x:c r="N7" s="7">
+        <x:v>1000</x:v>
+      </x:c>
+      <x:c r="O7" s="5">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="P7" s="7">
+        <x:f t="shared" si="1"/>
+        <x:v>1.1226892181772499</x:v>
+      </x:c>
+      <x:c r="Q7" s="6">
+        <x:f t="shared" si="2"/>
+        <x:v>0.6958499866549489</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="2:17">
       <x:c r="B8" s="15"/>
       <x:c r="C8" s="5">
         <x:v>3000</x:v>
@@ -1530,8 +1617,22 @@
       <x:c r="L8" s="6">
         <x:v>4183</x:v>
       </x:c>
-    </x:row>
-    <x:row r="9" spans="2:12">
+      <x:c r="N8" s="7">
+        <x:v>3000</x:v>
+      </x:c>
+      <x:c r="O8" s="5">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="P8" s="7">
+        <x:f t="shared" si="1"/>
+        <x:v>7.7788796670568301</x:v>
+      </x:c>
+      <x:c r="Q8" s="6">
+        <x:f t="shared" si="2"/>
+        <x:v>4.8213995688852833</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="2:17">
       <x:c r="B9" s="15"/>
       <x:c r="C9" s="5">
         <x:v>100</x:v>
@@ -1559,8 +1660,22 @@
       <x:c r="L9" s="6">
         <x:v>1658</x:v>
       </x:c>
-    </x:row>
-    <x:row r="10" spans="2:12">
+      <x:c r="N9" s="7">
+        <x:v>100</x:v>
+      </x:c>
+      <x:c r="O9" s="5">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="P9" s="7">
+        <x:f t="shared" si="1"/>
+        <x:v>0.016297083186294407</x:v>
+      </x:c>
+      <x:c r="Q9" s="6">
+        <x:f t="shared" si="2"/>
+        <x:v>0.010101036808841203</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="2:17">
       <x:c r="B10" s="15"/>
       <x:c r="C10" s="5">
         <x:v>300</x:v>
@@ -1588,8 +1703,22 @@
       <x:c r="L10" s="6">
         <x:v>2636</x:v>
       </x:c>
-    </x:row>
-    <x:row r="11" spans="2:12">
+      <x:c r="N10" s="7">
+        <x:v>300</x:v>
+      </x:c>
+      <x:c r="O10" s="5">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="P10" s="7">
+        <x:f t="shared" si="1"/>
+        <x:v>0.093045659880383463</x:v>
+      </x:c>
+      <x:c r="Q10" s="6">
+        <x:f t="shared" si="2"/>
+        <x:v>0.05767029747661092</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="2:17">
       <x:c r="B11" s="15"/>
       <x:c r="C11" s="5">
         <x:v>500</x:v>
@@ -1617,8 +1746,22 @@
       <x:c r="L11" s="6">
         <x:v>3122</x:v>
       </x:c>
-    </x:row>
-    <x:row r="12" spans="2:12">
+      <x:c r="N11" s="7">
+        <x:v>500</x:v>
+      </x:c>
+      <x:c r="O11" s="5">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="P11" s="7">
+        <x:f t="shared" si="1"/>
+        <x:v>0.18105514290860675</x:v>
+      </x:c>
+      <x:c r="Q11" s="6">
+        <x:f t="shared" si="2"/>
+        <x:v>0.11221914020098217</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="2:17">
       <x:c r="B12" s="15"/>
       <x:c r="C12" s="5">
         <x:v>1000</x:v>
@@ -1646,8 +1789,22 @@
       <x:c r="L12" s="6">
         <x:v>3673</x:v>
       </x:c>
-    </x:row>
-    <x:row r="13" spans="2:12" ht="14.550000000000001">
+      <x:c r="N12" s="7">
+        <x:v>1000</x:v>
+      </x:c>
+      <x:c r="O12" s="5">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="P12" s="7">
+        <x:f t="shared" si="1"/>
+        <x:v>0.62480929903472215</x:v>
+      </x:c>
+      <x:c r="Q12" s="6">
+        <x:f t="shared" si="2"/>
+        <x:v>0.38726081568778137</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="2:17" ht="14.550000000000001">
       <x:c r="B13" s="18"/>
       <x:c r="C13" s="19">
         <x:v>3000</x:v>
@@ -1675,10 +1832,24 @@
       <x:c r="L13" s="10">
         <x:v>4183</x:v>
       </x:c>
+      <x:c r="N13" s="31">
+        <x:v>3000</x:v>
+      </x:c>
+      <x:c r="O13" s="9">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="P13" s="31">
+        <x:f t="shared" si="1"/>
+        <x:v>2.6782625642608999</x:v>
+      </x:c>
+      <x:c r="Q13" s="10">
+        <x:f t="shared" si="2"/>
+        <x:v>1.6600043355053942</x:v>
+      </x:c>
     </x:row>
     <x:row r="14" spans="2:6">
       <x:c r="B14" s="15" t="s">
-        <x:v>16</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="C14" s="11"/>
       <x:c r="D14" s="11"/>
@@ -1688,16 +1859,16 @@
     <x:row r="15" spans="2:10" ht="14.550000000000001">
       <x:c r="B15" s="15"/>
       <x:c r="C15" s="5" t="s">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="D15" s="5" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E15" s="5" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="F15" s="16" t="s">
         <x:v>7</x:v>
-      </x:c>
-      <x:c r="E15" s="5" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="F15" s="16" t="s">
-        <x:v>3</x:v>
       </x:c>
       <x:c r="H15" s="21" t="s">
         <x:v>5</x:v>
@@ -1721,10 +1892,10 @@
       </x:c>
       <x:c r="H16" s="24"/>
       <x:c r="I16" s="5" t="s">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="J16" s="25" t="s">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="2:10">
@@ -1914,16 +2085,16 @@
     <x:row r="27" spans="2:6">
       <x:c r="B27" s="15"/>
       <x:c r="C27" s="5" t="s">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="D27" s="5" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E27" s="5" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="F27" s="16" t="s">
         <x:v>7</x:v>
-      </x:c>
-      <x:c r="E27" s="5" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="F27" s="16" t="s">
-        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="28" spans="2:6">
@@ -2078,7 +2249,7 @@
     </x:row>
     <x:row r="38" spans="2:6">
       <x:c r="B38" s="15" t="s">
-        <x:v>13</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C38" s="11"/>
       <x:c r="D38" s="11"/>
@@ -2088,16 +2259,16 @@
     <x:row r="39" spans="2:6">
       <x:c r="B39" s="15"/>
       <x:c r="C39" s="5" t="s">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="D39" s="5" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E39" s="5" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="F39" s="16" t="s">
         <x:v>7</x:v>
-      </x:c>
-      <x:c r="E39" s="5" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="F39" s="16" t="s">
-        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="2:6">
@@ -2252,7 +2423,7 @@
     </x:row>
     <x:row r="50" spans="2:6">
       <x:c r="B50" s="15" t="s">
-        <x:v>14</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C50" s="11"/>
       <x:c r="D50" s="11"/>
@@ -2262,16 +2433,16 @@
     <x:row r="51" spans="2:6">
       <x:c r="B51" s="15"/>
       <x:c r="C51" s="5" t="s">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="D51" s="5" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E51" s="5" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="F51" s="16" t="s">
         <x:v>7</x:v>
-      </x:c>
-      <x:c r="E51" s="5" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="F51" s="16" t="s">
-        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="2:6">
@@ -2426,7 +2597,7 @@
     </x:row>
     <x:row r="62" spans="2:6">
       <x:c r="B62" s="15" t="s">
-        <x:v>6</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C62" s="11"/>
       <x:c r="D62" s="11"/>
@@ -2436,16 +2607,16 @@
     <x:row r="63" spans="2:6">
       <x:c r="B63" s="15"/>
       <x:c r="C63" s="5" t="s">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="D63" s="5" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E63" s="5" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="F63" s="16" t="s">
         <x:v>7</x:v>
-      </x:c>
-      <x:c r="E63" s="5" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="F63" s="16" t="s">
-        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="64" spans="2:6">
@@ -2600,7 +2771,7 @@
     </x:row>
     <x:row r="74" spans="2:6">
       <x:c r="B74" s="15" t="s">
-        <x:v>15</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="C74" s="11"/>
       <x:c r="D74" s="11"/>
@@ -2610,16 +2781,16 @@
     <x:row r="75" spans="2:6">
       <x:c r="B75" s="15"/>
       <x:c r="C75" s="5" t="s">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="D75" s="5" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E75" s="5" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="F75" s="16" t="s">
         <x:v>7</x:v>
-      </x:c>
-      <x:c r="E75" s="5" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="F75" s="16" t="s">
-        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="76" spans="2:6">
@@ -2774,7 +2945,7 @@
     </x:row>
     <x:row r="86" spans="2:6">
       <x:c r="B86" s="15" t="s">
-        <x:v>9</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="C86" s="11"/>
       <x:c r="D86" s="11"/>
@@ -2784,16 +2955,16 @@
     <x:row r="87" spans="2:6">
       <x:c r="B87" s="15"/>
       <x:c r="C87" s="5" t="s">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="D87" s="5" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E87" s="5" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="F87" s="16" t="s">
         <x:v>7</x:v>
-      </x:c>
-      <x:c r="E87" s="5" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="F87" s="16" t="s">
-        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="88" spans="2:6">
@@ -2948,7 +3119,7 @@
     </x:row>
     <x:row r="98" spans="2:6">
       <x:c r="B98" s="15" t="s">
-        <x:v>8</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="C98" s="11"/>
       <x:c r="D98" s="11"/>
@@ -2958,16 +3129,16 @@
     <x:row r="99" spans="2:6">
       <x:c r="B99" s="15"/>
       <x:c r="C99" s="5" t="s">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="D99" s="5" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E99" s="5" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="F99" s="16" t="s">
         <x:v>7</x:v>
-      </x:c>
-      <x:c r="E99" s="5" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="F99" s="16" t="s">
-        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="100" spans="2:6">
@@ -3122,7 +3293,7 @@
     </x:row>
     <x:row r="110" spans="2:6">
       <x:c r="B110" s="15" t="s">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="C110" s="11"/>
       <x:c r="D110" s="11"/>
@@ -3132,16 +3303,16 @@
     <x:row r="111" spans="2:6">
       <x:c r="B111" s="15"/>
       <x:c r="C111" s="5" t="s">
-        <x:v>0</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="D111" s="5" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E111" s="5" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="F111" s="16" t="s">
         <x:v>7</x:v>
-      </x:c>
-      <x:c r="E111" s="5" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="F111" s="16" t="s">
-        <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="112" spans="2:6">

</xml_diff>